<commit_message>
Base para consulta com os dados corrigidos agora, valores de 2022 devidamente atualizados
</commit_message>
<xml_diff>
--- a/baseDados/basesLimpas.xlsx
+++ b/baseDados/basesLimpas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\51520717890\Documents\GitHub\Waste-Data-SP\baseDados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031D7583-30D7-44FB-9EE0-333671FDDBD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F86EB6-1FF6-46DD-AF25-BFC5117C01FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,12 +111,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,7 +423,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="A2:L13"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,8 +500,8 @@
       <c r="I2" s="2">
         <v>308771.34000000003</v>
       </c>
-      <c r="J2" s="2">
-        <v>295133.44</v>
+      <c r="J2">
+        <v>299226.13</v>
       </c>
       <c r="K2" s="2">
         <v>295133.44</v>
@@ -537,8 +538,8 @@
       <c r="I3" s="2">
         <v>278865.96000000002</v>
       </c>
-      <c r="J3" s="2">
-        <v>276302.21000000002</v>
+      <c r="J3">
+        <v>274821.67</v>
       </c>
       <c r="K3" s="2">
         <v>276302.21000000002</v>
@@ -575,8 +576,8 @@
       <c r="I4" s="2">
         <v>314020.61</v>
       </c>
-      <c r="J4" s="2">
-        <v>306021.76000000001</v>
+      <c r="J4">
+        <v>305662.03999999998</v>
       </c>
       <c r="K4" s="2">
         <v>306021.76000000001</v>
@@ -613,8 +614,8 @@
       <c r="I5" s="2">
         <v>274942.26</v>
       </c>
-      <c r="J5" s="2">
-        <v>266533.19</v>
+      <c r="J5">
+        <v>275167.42</v>
       </c>
       <c r="K5" s="2">
         <v>266533.19</v>
@@ -651,8 +652,8 @@
       <c r="I6" s="2">
         <v>277720.63</v>
       </c>
-      <c r="J6" s="2">
-        <v>288978.31</v>
+      <c r="J6">
+        <v>276489.61</v>
       </c>
       <c r="K6" s="2">
         <v>288978.31</v>
@@ -689,8 +690,8 @@
       <c r="I7" s="2">
         <v>276873.3</v>
       </c>
-      <c r="J7" s="2">
-        <v>273364.94</v>
+      <c r="J7">
+        <v>270059.27</v>
       </c>
       <c r="K7" s="2">
         <v>273364.94</v>
@@ -727,8 +728,8 @@
       <c r="I8" s="2">
         <v>275104.11</v>
       </c>
-      <c r="J8" s="2">
-        <v>276232.8</v>
+      <c r="J8">
+        <v>265810.43</v>
       </c>
       <c r="K8" s="2">
         <v>276232.8</v>
@@ -765,8 +766,8 @@
       <c r="I9" s="2">
         <v>281445.44</v>
       </c>
-      <c r="J9" s="2">
-        <v>290545.02</v>
+      <c r="J9">
+        <v>280041.17</v>
       </c>
       <c r="K9" s="2">
         <v>290545.02</v>
@@ -803,8 +804,8 @@
       <c r="I10" s="2">
         <v>273401.23</v>
       </c>
-      <c r="J10" s="2">
-        <v>281255.24</v>
+      <c r="J10">
+        <v>259983.59</v>
       </c>
       <c r="K10" s="2">
         <v>281255.24</v>
@@ -841,8 +842,8 @@
       <c r="I11" s="2">
         <v>275099.12</v>
       </c>
-      <c r="J11" s="2">
-        <v>297534.7</v>
+      <c r="J11">
+        <v>283615.59000000003</v>
       </c>
       <c r="K11" s="2">
         <v>297534.7</v>
@@ -879,8 +880,8 @@
       <c r="I12" s="2">
         <v>285569.11</v>
       </c>
-      <c r="J12" s="2">
-        <v>293825.90000000002</v>
+      <c r="J12">
+        <v>277227.8</v>
       </c>
       <c r="K12" s="2">
         <v>293825.90000000002</v>
@@ -917,8 +918,8 @@
       <c r="I13" s="2">
         <v>299566.33</v>
       </c>
-      <c r="J13" s="2">
-        <v>307069.36</v>
+      <c r="J13" s="3">
+        <v>306083.39</v>
       </c>
       <c r="K13" s="2">
         <v>307069.36</v>
@@ -929,6 +930,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A1:L1" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>